<commit_message>
dev: make some changes
</commit_message>
<xml_diff>
--- a/Codigo/backend/src/main/java/amplasystem/api/out/purchaseOrdersReport.xlsx
+++ b/Codigo/backend/src/main/java/amplasystem/api/out/purchaseOrdersReport.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>ID</t>
   </si>
@@ -63,6 +63,21 @@
   </si>
   <si>
     <t>NAOFATURADO</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>123213</t>
+  </si>
+  <si>
+    <t>Cliente Pedro 1</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>TOTALMENTEFATURADO</t>
   </si>
 </sst>
 </file>
@@ -107,7 +122,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -159,10 +174,10 @@
         <v>123213.0</v>
       </c>
       <c r="G2" t="n" s="0">
-        <v>369.0</v>
+        <v>22468.0</v>
       </c>
       <c r="H2" t="n" s="0">
-        <v>36.900000000000006</v>
+        <v>2246.8</v>
       </c>
     </row>
     <row r="3">
@@ -189,6 +204,32 @@
       </c>
       <c r="H3" t="n" s="0">
         <v>0.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="F4" t="n" s="0">
+        <v>200001.0</v>
+      </c>
+      <c r="G4" t="n" s="0">
+        <v>200001.0</v>
+      </c>
+      <c r="H4" t="n" s="0">
+        <v>9000.045</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: some erros and add new export function
</commit_message>
<xml_diff>
--- a/Codigo/backend/src/main/java/amplasystem/api/out/purchaseOrdersReport.xlsx
+++ b/Codigo/backend/src/main/java/amplasystem/api/out/purchaseOrdersReport.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <t>ID</t>
   </si>
@@ -62,9 +62,6 @@
     <t>1232132132111</t>
   </si>
   <si>
-    <t>NAOFATURADO</t>
-  </si>
-  <si>
     <t>4</t>
   </si>
   <si>
@@ -78,13 +75,21 @@
   </si>
   <si>
     <t>TOTALMENTEFATURADO</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>33333333a</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="R$ #,##0.00"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <sz val="11.0"/>
@@ -114,19 +119,41 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="2.640625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="14.00390625" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="14.8984375" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="15.01953125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="22.5390625" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="13.14453125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="12.4375" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="15.25390625" customWidth="true" bestFit="true"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
@@ -170,14 +197,14 @@
       <c r="E2" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="F2" t="n" s="0">
+      <c r="F2" t="n" s="1">
         <v>123213.0</v>
       </c>
-      <c r="G2" t="n" s="0">
-        <v>22468.0</v>
-      </c>
-      <c r="H2" t="n" s="0">
-        <v>2246.8</v>
+      <c r="G2" t="n" s="2">
+        <v>22714.21</v>
+      </c>
+      <c r="H2" t="n" s="3">
+        <v>2271.4210000000003</v>
       </c>
     </row>
     <row r="3">
@@ -194,42 +221,68 @@
         <v>15</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>16</v>
-      </c>
-      <c r="F3" t="n" s="0">
+        <v>12</v>
+      </c>
+      <c r="F3" t="n" s="4">
         <v>123213.0</v>
       </c>
-      <c r="G3" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="H3" t="n" s="0">
-        <v>0.0</v>
+      <c r="G3" t="n" s="5">
+        <v>12743.0</v>
+      </c>
+      <c r="H3" t="n" s="6">
+        <v>1274.3000000000002</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="C4" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="D4" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="D4" t="s" s="0">
+      <c r="E4" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="E4" t="s" s="0">
+      <c r="F4" t="n" s="7">
+        <v>200001.0</v>
+      </c>
+      <c r="G4" t="n" s="8">
+        <v>200001.0</v>
+      </c>
+      <c r="H4" t="n" s="9">
+        <v>9000.045</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
         <v>21</v>
       </c>
-      <c r="F4" t="n" s="0">
-        <v>200001.0</v>
-      </c>
-      <c r="G4" t="n" s="0">
-        <v>200001.0</v>
-      </c>
-      <c r="H4" t="n" s="0">
-        <v>9000.045</v>
+      <c r="B5" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="F5" t="n" s="10">
+        <v>200.0</v>
+      </c>
+      <c r="G5" t="n" s="11">
+        <v>200.0</v>
+      </c>
+      <c r="H5" t="n" s="12">
+        <v>20.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>